<commit_message>
increase HIV muliplier on HPV infection
</commit_message>
<xml_diff>
--- a/Config/HIV_parameters_Kenya.xlsx
+++ b/Config/HIV_parameters_Kenya.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20358"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Kenya_model_Feb20\HHCoM\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Kenya_model_Feb20\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AAF2CD-7B21-4419-86CF-138F32C3B1B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19620" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Protection" sheetId="5" r:id="rId1"/>
     <sheet name="Disease Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="87">
   <si>
     <t>Male</t>
   </si>
@@ -306,11 +306,14 @@
   <si>
     <t>Original values</t>
   </si>
+  <si>
+    <t xml:space="preserve">original values </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1004,12 +1007,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AI51"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2368,6 +2371,9 @@
       <c r="G41" s="14">
         <v>9</v>
       </c>
+      <c r="H41" t="s">
+        <v>86</v>
+      </c>
       <c r="J41" s="68"/>
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
@@ -2394,11 +2400,12 @@
         <v>2013</v>
       </c>
       <c r="B42" s="69">
-        <v>49.3996</v>
+        <f>H42-5</f>
+        <v>44.4</v>
       </c>
       <c r="C42" s="64">
         <f t="shared" si="0"/>
-        <v>36.555703999999999</v>
+        <v>32.856000000000002</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>75</v>
@@ -2409,7 +2416,21 @@
       <c r="G42" s="9">
         <v>10</v>
       </c>
+      <c r="H42" s="14">
+        <v>49.4</v>
+      </c>
+      <c r="I42" s="14">
+        <v>36.555703999999999</v>
+      </c>
       <c r="J42" s="68"/>
+      <c r="L42">
+        <f>H42-5</f>
+        <v>44.4</v>
+      </c>
+      <c r="M42" s="14">
+        <f>I42-5</f>
+        <v>31.555703999999999</v>
+      </c>
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
       <c r="S42" s="4"/>
@@ -2434,8 +2455,9 @@
       <c r="A43" s="70">
         <v>2015</v>
       </c>
-      <c r="B43" s="64">
-        <v>49.764000000000003</v>
+      <c r="B43" s="69">
+        <f t="shared" ref="B43:B46" si="1">H43-5</f>
+        <v>44.764000000000003</v>
       </c>
       <c r="C43" s="64">
         <v>38.454000000000001</v>
@@ -2449,7 +2471,21 @@
       <c r="G43" s="14">
         <v>11</v>
       </c>
+      <c r="H43" s="14">
+        <v>49.764000000000003</v>
+      </c>
+      <c r="I43" s="14">
+        <v>38.454000000000001</v>
+      </c>
       <c r="J43" s="68"/>
+      <c r="L43" s="14">
+        <f t="shared" ref="L43:L46" si="2">H43-5</f>
+        <v>44.764000000000003</v>
+      </c>
+      <c r="M43" s="14">
+        <f t="shared" ref="M43:M46" si="3">I43-5</f>
+        <v>33.454000000000001</v>
+      </c>
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
       <c r="S43" s="4"/>
@@ -2474,8 +2510,9 @@
       <c r="A44" s="70">
         <v>2016</v>
       </c>
-      <c r="B44" s="64">
-        <v>59.2</v>
+      <c r="B44" s="69">
+        <f t="shared" si="1"/>
+        <v>54.2</v>
       </c>
       <c r="C44" s="64">
         <v>44.800000000000004</v>
@@ -2488,6 +2525,20 @@
       </c>
       <c r="G44" s="14">
         <v>12</v>
+      </c>
+      <c r="H44" s="14">
+        <v>59.2</v>
+      </c>
+      <c r="I44" s="14">
+        <v>44.8</v>
+      </c>
+      <c r="L44" s="14">
+        <f t="shared" si="2"/>
+        <v>54.2</v>
+      </c>
+      <c r="M44" s="14">
+        <f t="shared" si="3"/>
+        <v>39.799999999999997</v>
       </c>
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
@@ -2513,8 +2564,9 @@
       <c r="A45" s="70">
         <v>2017</v>
       </c>
-      <c r="B45" s="64">
-        <v>68</v>
+      <c r="B45" s="69">
+        <f t="shared" si="1"/>
+        <v>63</v>
       </c>
       <c r="C45" s="64">
         <v>51.85</v>
@@ -2527,6 +2579,20 @@
       </c>
       <c r="G45" s="9">
         <v>13</v>
+      </c>
+      <c r="H45" s="14">
+        <v>68</v>
+      </c>
+      <c r="I45" s="14">
+        <v>51.85</v>
+      </c>
+      <c r="L45" s="14">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="M45" s="14">
+        <f t="shared" si="3"/>
+        <v>46.85</v>
       </c>
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
@@ -2552,8 +2618,9 @@
       <c r="A46" s="70">
         <v>2018</v>
       </c>
-      <c r="B46" s="13">
-        <v>67.95</v>
+      <c r="B46" s="69">
+        <f t="shared" si="1"/>
+        <v>62.95</v>
       </c>
       <c r="C46" s="13">
         <v>53.631</v>
@@ -2566,6 +2633,20 @@
       </c>
       <c r="G46" s="14">
         <v>14</v>
+      </c>
+      <c r="H46" s="14">
+        <v>67.95</v>
+      </c>
+      <c r="I46" s="14">
+        <v>53.631</v>
+      </c>
+      <c r="L46" s="14">
+        <f t="shared" si="2"/>
+        <v>62.95</v>
+      </c>
+      <c r="M46" s="14">
+        <f t="shared" si="3"/>
+        <v>48.631</v>
       </c>
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
@@ -2710,11 +2791,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AX187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -9110,7 +9191,7 @@
     <mergeCell ref="H45:H60"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C8" r:id="rId1" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4790087/"/>
+    <hyperlink ref="C8" r:id="rId1" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4790087/" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Increase mue2 and mue3 to fit UN pop data
</commit_message>
<xml_diff>
--- a/Config/HIV_parameters_Kenya.xlsx
+++ b/Config/HIV_parameters_Kenya.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20363"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20364"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Kenya_model_HPV-HIVacq\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD32640-1E74-4DAD-B87D-37480299D736}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968F9791-A00C-4538-A7E9-605E66BE1F17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19215" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="5955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Protection" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="91">
   <si>
     <t>Male</t>
   </si>
@@ -277,9 +277,6 @@
     <t>AIDS progress report 2016, VS% from KAIS 2012</t>
   </si>
   <si>
-    <t>Gargano, et al</t>
-  </si>
-  <si>
     <t>UNAIDS estimate, VS% from PHIA</t>
   </si>
   <si>
@@ -319,9 +316,6 @@
     <t>* VS% = 75% of reported ART coverage among all PLHIV, based on KAIS 2012</t>
   </si>
   <si>
-    <t>Baeten JM, Donnell D, Kapiga SH, et al. Male circumcision and risk of male-to-female HIV-1 transmission: a multinational prospective study in African HIV-1-serodiscordant couples. AIDS. 2010;24(5):737-744.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <i/>
@@ -342,14 +336,16 @@
       <t>. Male circumcision and risk of male-to-female HIV-1 transmission: a multinational prospective study in African HIV-1-serodiscordant couples. AIDS. 2010;24(5):737-744.</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve"> Kenya HIV estimates, 2018</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -586,7 +582,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -715,10 +711,11 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -755,8 +752,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1044,10 +1039,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:AI62"/>
+  <dimension ref="A1:AI66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,7 +1097,7 @@
     </row>
     <row r="2" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -1316,9 +1311,9 @@
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
@@ -1387,7 +1382,7 @@
     </row>
     <row r="11" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
@@ -1947,23 +1942,23 @@
       <c r="AI29" s="4"/>
     </row>
     <row r="30" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="72" t="s">
+      <c r="A30" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="72"/>
-      <c r="C30" s="72"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="72"/>
-      <c r="F30" s="72"/>
-      <c r="G30" s="72"/>
-      <c r="H30" s="72"/>
-      <c r="I30" s="72"/>
-      <c r="J30" s="72"/>
-      <c r="K30" s="72"/>
-      <c r="L30" s="72"/>
-      <c r="M30" s="72"/>
-      <c r="N30" s="72"/>
-      <c r="O30" s="72"/>
+      <c r="B30" s="73"/>
+      <c r="C30" s="73"/>
+      <c r="D30" s="73"/>
+      <c r="E30" s="73"/>
+      <c r="F30" s="73"/>
+      <c r="G30" s="73"/>
+      <c r="H30" s="73"/>
+      <c r="I30" s="73"/>
+      <c r="J30" s="73"/>
+      <c r="K30" s="73"/>
+      <c r="L30" s="73"/>
+      <c r="M30" s="73"/>
+      <c r="N30" s="73"/>
+      <c r="O30" s="73"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
@@ -1985,23 +1980,23 @@
       <c r="AI30" s="4"/>
     </row>
     <row r="31" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="73" t="s">
+      <c r="A31" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="73"/>
-      <c r="H31" s="73"/>
-      <c r="I31" s="73"/>
-      <c r="J31" s="73"/>
-      <c r="K31" s="73"/>
-      <c r="L31" s="73"/>
-      <c r="M31" s="73"/>
-      <c r="N31" s="73"/>
-      <c r="O31" s="73"/>
+      <c r="B31" s="74"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="74"/>
+      <c r="I31" s="74"/>
+      <c r="J31" s="74"/>
+      <c r="K31" s="74"/>
+      <c r="L31" s="74"/>
+      <c r="M31" s="74"/>
+      <c r="N31" s="74"/>
+      <c r="O31" s="74"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
       <c r="S31" s="4"/>
@@ -2033,7 +2028,7 @@
         <v>71</v>
       </c>
       <c r="L32" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M32" s="14" t="s">
         <v>1</v>
@@ -2042,7 +2037,7 @@
         <v>0</v>
       </c>
       <c r="O32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
@@ -2074,8 +2069,8 @@
       <c r="C33" s="64">
         <v>0</v>
       </c>
-      <c r="D33" t="s">
-        <v>76</v>
+      <c r="D33" s="14" t="s">
+        <v>90</v>
       </c>
       <c r="F33" s="14">
         <v>2003</v>
@@ -2089,14 +2084,14 @@
       <c r="L33" s="14">
         <v>2004</v>
       </c>
-      <c r="M33" s="84">
-        <v>1.3083920290325319</v>
-      </c>
-      <c r="N33" s="84">
-        <v>1.6980612730897779</v>
+      <c r="M33" s="14">
+        <v>0.87226135268835459</v>
+      </c>
+      <c r="N33" s="14">
+        <v>1.1320408487265186</v>
       </c>
       <c r="O33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
@@ -2122,15 +2117,15 @@
       <c r="A34" s="64">
         <v>2005</v>
       </c>
-      <c r="B34" s="69">
-        <v>0.11943150603129105</v>
+      <c r="B34" s="68">
+        <v>2.9059037050679932</v>
       </c>
       <c r="C34" s="64">
         <f t="shared" ref="C34:C42" si="0">0.74*B34</f>
-        <v>8.8379314463155376E-2</v>
+        <v>2.1503687417503148</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="F34" s="14">
         <v>2004</v>
@@ -2144,11 +2139,11 @@
       <c r="L34" s="14">
         <v>2005</v>
       </c>
-      <c r="M34" s="84">
+      <c r="M34" s="14">
         <v>2.9059037050679932</v>
       </c>
-      <c r="N34" s="84">
-        <v>3.7967333204294031</v>
+      <c r="N34" s="14">
+        <v>2.5311555469529354</v>
       </c>
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
@@ -2174,15 +2169,15 @@
       <c r="A35" s="64">
         <v>2006</v>
       </c>
-      <c r="B35" s="69">
-        <v>1.0854341736694677</v>
+      <c r="B35" s="68">
+        <v>6.5665006973826721</v>
       </c>
       <c r="C35" s="64">
         <f t="shared" si="0"/>
-        <v>0.80322128851540608</v>
+        <v>4.8592105160631771</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="F35" s="14">
         <v>2005</v>
@@ -2196,11 +2191,11 @@
       <c r="L35" s="14">
         <v>2006</v>
       </c>
-      <c r="M35" s="84">
+      <c r="M35" s="14">
         <v>6.5665006973826721</v>
       </c>
-      <c r="N35" s="84">
-        <v>8.6200480817215688</v>
+      <c r="N35" s="14">
+        <v>5.7466987211477125</v>
       </c>
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
@@ -2226,15 +2221,15 @@
       <c r="A36" s="64">
         <v>2007</v>
       </c>
-      <c r="B36" s="69">
-        <v>4.7345437830383821</v>
+      <c r="B36" s="68">
+        <v>9.1957070887825481</v>
       </c>
       <c r="C36" s="64">
         <f t="shared" si="0"/>
-        <v>3.5035623994484029</v>
+        <v>6.8048232456990858</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="F36" s="14">
         <v>2006</v>
@@ -2248,11 +2243,11 @@
       <c r="L36" s="14">
         <v>2007</v>
       </c>
-      <c r="M36" s="84">
+      <c r="M36" s="14">
         <v>9.1957070887825481</v>
       </c>
-      <c r="N36" s="84">
-        <v>12.094549993791215</v>
+      <c r="N36" s="14">
+        <v>8.063033329194143</v>
       </c>
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
@@ -2278,15 +2273,15 @@
       <c r="A37" s="64">
         <v>2008</v>
       </c>
-      <c r="B37" s="69">
-        <v>8.0786986150802385</v>
+      <c r="B37" s="68">
+        <v>12.503557954551336</v>
       </c>
       <c r="C37" s="64">
         <f t="shared" si="0"/>
-        <v>5.9782369751593762</v>
+        <v>9.252632886367989</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="F37" s="14">
         <v>2007</v>
@@ -2300,11 +2295,11 @@
       <c r="L37" s="14">
         <v>2008</v>
       </c>
-      <c r="M37" s="84">
+      <c r="M37" s="14">
         <v>12.503557954551336</v>
       </c>
-      <c r="N37" s="84">
-        <v>16.440054062132464</v>
+      <c r="N37" s="14">
+        <v>10.960036041421644</v>
       </c>
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
@@ -2330,7 +2325,7 @@
       <c r="A38" s="64">
         <v>2009</v>
       </c>
-      <c r="B38" s="69">
+      <c r="B38" s="68">
         <v>23.03933533384064</v>
       </c>
       <c r="C38" s="64">
@@ -2352,11 +2347,11 @@
       <c r="L38" s="14">
         <v>2009</v>
       </c>
-      <c r="M38" s="84">
+      <c r="M38" s="14">
         <v>16.96536733473387</v>
       </c>
-      <c r="N38" s="84">
-        <v>22.220695539853899</v>
+      <c r="N38" s="14">
+        <v>14.813797026569265</v>
       </c>
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
@@ -2382,7 +2377,7 @@
       <c r="A39" s="64">
         <v>2010</v>
       </c>
-      <c r="B39" s="69">
+      <c r="B39" s="68">
         <v>31.39083758325436</v>
       </c>
       <c r="C39" s="64">
@@ -2398,15 +2393,16 @@
       <c r="G39" s="9">
         <v>7</v>
       </c>
-      <c r="J39" s="68"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
       <c r="L39" s="14">
         <v>2010</v>
       </c>
-      <c r="M39" s="84">
-        <v>22.691288338593512</v>
-      </c>
-      <c r="N39" s="84">
-        <v>27.1560777865852</v>
+      <c r="M39" s="14">
+        <v>19.665783226781045</v>
+      </c>
+      <c r="N39" s="14">
+        <v>19.914457043495815</v>
       </c>
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
@@ -2432,7 +2428,7 @@
       <c r="A40" s="64">
         <v>2011</v>
       </c>
-      <c r="B40" s="69">
+      <c r="B40" s="68">
         <v>35.323435905602842</v>
       </c>
       <c r="C40" s="64">
@@ -2448,15 +2444,16 @@
       <c r="G40" s="14">
         <v>8</v>
       </c>
-      <c r="J40" s="68"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
       <c r="L40" s="14">
         <v>2011</v>
       </c>
-      <c r="M40" s="84">
-        <v>32.132830803033713</v>
-      </c>
-      <c r="N40" s="84">
-        <v>25.676713341272123</v>
+      <c r="M40" s="14">
+        <v>27.848453362629218</v>
+      </c>
+      <c r="N40" s="14">
+        <v>20.541370673017699</v>
       </c>
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
@@ -2482,7 +2479,7 @@
       <c r="A41" s="64">
         <v>2012</v>
       </c>
-      <c r="B41" s="69">
+      <c r="B41" s="68">
         <v>38.706882519484815</v>
       </c>
       <c r="C41" s="64">
@@ -2499,17 +2496,18 @@
         <v>9</v>
       </c>
       <c r="H41" t="s">
-        <v>86</v>
-      </c>
-      <c r="J41" s="68"/>
+        <v>85</v>
+      </c>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
       <c r="L41" s="14">
         <v>2012</v>
       </c>
-      <c r="M41" s="84">
+      <c r="M41" s="14">
         <v>35.042296598850157</v>
       </c>
-      <c r="N41" s="84">
-        <v>28.132598451801307</v>
+      <c r="N41" s="14">
+        <v>26.257091888347887</v>
       </c>
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
@@ -2535,13 +2533,13 @@
       <c r="A42" s="64">
         <v>2013</v>
       </c>
-      <c r="B42" s="69">
+      <c r="B42" s="68">
         <f>H42-5</f>
         <v>44.4</v>
       </c>
       <c r="C42" s="64">
-        <f t="shared" si="0"/>
-        <v>32.856000000000002</v>
+        <f>I42</f>
+        <v>36.555703999999999</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>75</v>
@@ -2558,15 +2556,16 @@
       <c r="I42" s="14">
         <v>36.555703999999999</v>
       </c>
-      <c r="J42" s="68"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
       <c r="L42" s="14">
         <v>2013</v>
       </c>
-      <c r="M42" s="84">
+      <c r="M42" s="14">
         <v>37.664670733960989</v>
       </c>
-      <c r="N42" s="84">
-        <v>29.252699938151203</v>
+      <c r="N42" s="14">
+        <v>27.302519942274454</v>
       </c>
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
@@ -2589,10 +2588,10 @@
       <c r="AI42" s="4"/>
     </row>
     <row r="43" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="70">
+      <c r="A43" s="69">
         <v>2015</v>
       </c>
-      <c r="B43" s="69">
+      <c r="B43" s="68">
         <f t="shared" ref="B43:B46" si="1">H43-5</f>
         <v>44.764000000000003</v>
       </c>
@@ -2600,7 +2599,7 @@
         <v>38.454000000000001</v>
       </c>
       <c r="D43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F43" s="14">
         <v>2014</v>
@@ -2614,15 +2613,16 @@
       <c r="I43" s="14">
         <v>38.454000000000001</v>
       </c>
-      <c r="J43" s="68"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
       <c r="L43" s="14">
         <v>2015</v>
       </c>
-      <c r="M43" s="84">
-        <v>50.73423033275192</v>
-      </c>
-      <c r="N43" s="84">
-        <v>38.233815949870618</v>
+      <c r="M43" s="14">
+        <v>43.387743936920174</v>
+      </c>
+      <c r="N43" s="14">
+        <v>29.872884348296882</v>
       </c>
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
@@ -2645,10 +2645,10 @@
       <c r="AI43" s="4"/>
     </row>
     <row r="44" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="70">
+      <c r="A44" s="69">
         <v>2016</v>
       </c>
-      <c r="B44" s="69">
+      <c r="B44" s="68">
         <f t="shared" si="1"/>
         <v>54.2</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>44.800000000000004</v>
       </c>
       <c r="D44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F44" s="14">
         <v>2015</v>
@@ -2670,14 +2670,16 @@
       <c r="I44" s="14">
         <v>44.8</v>
       </c>
+      <c r="J44" s="14"/>
+      <c r="K44" s="14"/>
       <c r="L44" s="14">
         <v>2016</v>
       </c>
-      <c r="M44" s="84">
-        <v>57.224897163583051</v>
-      </c>
-      <c r="N44" s="84">
-        <v>41.913057767373743</v>
+      <c r="M44" s="14">
+        <v>50.73423033275192</v>
+      </c>
+      <c r="N44" s="14">
+        <v>35.684894886545912</v>
       </c>
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
@@ -2700,10 +2702,10 @@
       <c r="AI44" s="4"/>
     </row>
     <row r="45" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="70">
+      <c r="A45" s="69">
         <v>2017</v>
       </c>
-      <c r="B45" s="69">
+      <c r="B45" s="68">
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
@@ -2711,7 +2713,7 @@
         <v>51.85</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F45" s="14">
         <v>2016</v>
@@ -2725,14 +2727,16 @@
       <c r="I45" s="14">
         <v>51.85</v>
       </c>
+      <c r="J45" s="14"/>
+      <c r="K45" s="4"/>
       <c r="L45" s="14">
         <v>2017</v>
       </c>
-      <c r="M45" s="84">
-        <v>61.893808574842218</v>
-      </c>
-      <c r="N45" s="84">
-        <v>46.140623298934813</v>
+      <c r="M45" s="4">
+        <v>57.224897163583051</v>
+      </c>
+      <c r="N45" s="4">
+        <v>39.118853916215492</v>
       </c>
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
@@ -2755,10 +2759,10 @@
       <c r="AI45" s="4"/>
     </row>
     <row r="46" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="70">
+      <c r="A46" s="69">
         <v>2018</v>
       </c>
-      <c r="B46" s="69">
+      <c r="B46" s="68">
         <f t="shared" si="1"/>
         <v>62.95</v>
       </c>
@@ -2766,7 +2770,7 @@
         <v>53.631</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F46" s="14">
         <v>2017</v>
@@ -2780,14 +2784,16 @@
       <c r="I46" s="14">
         <v>53.631</v>
       </c>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
       <c r="L46">
         <v>2018</v>
       </c>
-      <c r="M46">
-        <v>62.95</v>
-      </c>
-      <c r="N46">
-        <v>53.631</v>
+      <c r="M46" s="4">
+        <v>61.893808574842218</v>
+      </c>
+      <c r="N46" s="4">
+        <v>43.064581745672491</v>
       </c>
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
@@ -2867,7 +2873,7 @@
       <c r="C49">
         <v>1.6980612730897779</v>
       </c>
-      <c r="D49" s="84">
+      <c r="D49" s="71">
         <v>1.3083920290325319</v>
       </c>
       <c r="Q49" s="4"/>
@@ -2900,21 +2906,11 @@
       <c r="C50">
         <v>3.7967333204294031</v>
       </c>
-      <c r="D50" s="84">
+      <c r="D50" s="71">
         <v>2.9059037050679932</v>
       </c>
-      <c r="L50" s="14">
-        <v>2014</v>
-      </c>
-      <c r="M50" s="84">
-        <v>43.387743936920174</v>
-      </c>
-      <c r="N50" s="84">
-        <v>32.00666180174666</v>
-      </c>
-      <c r="Q50" s="4"/>
-      <c r="R50" s="4"/>
-      <c r="S50" s="4"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
       <c r="T50" s="4"/>
       <c r="U50" s="4"/>
       <c r="V50" s="4"/>
@@ -2942,9 +2938,15 @@
       <c r="C51">
         <v>8.6200480817215688</v>
       </c>
-      <c r="D51" s="84">
+      <c r="D51" s="71">
         <v>6.5665006973826721</v>
       </c>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="71"/>
+      <c r="N51" s="71"/>
       <c r="Q51" s="4"/>
       <c r="R51" s="4"/>
       <c r="S51" s="4"/>
@@ -2975,9 +2977,12 @@
       <c r="C52">
         <v>12.094549993791215</v>
       </c>
-      <c r="D52" s="84">
+      <c r="D52" s="71">
         <v>9.1957070887825481</v>
       </c>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
     </row>
     <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53">
@@ -2989,9 +2994,14 @@
       <c r="C53">
         <v>16.440054062132464</v>
       </c>
-      <c r="D53" s="84">
+      <c r="D53" s="71">
         <v>12.503557954551336</v>
       </c>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
     </row>
     <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54">
@@ -3003,9 +3013,14 @@
       <c r="C54">
         <v>22.220695539853899</v>
       </c>
-      <c r="D54" s="84">
+      <c r="D54" s="71">
         <v>16.96536733473387</v>
       </c>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
     </row>
     <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55">
@@ -3017,9 +3032,14 @@
       <c r="C55">
         <v>27.1560777865852</v>
       </c>
-      <c r="D55" s="84">
+      <c r="D55" s="71">
         <v>22.691288338593512</v>
       </c>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
     </row>
     <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56">
@@ -3031,9 +3051,14 @@
       <c r="C56">
         <v>25.676713341272123</v>
       </c>
-      <c r="D56" s="84">
+      <c r="D56" s="71">
         <v>32.132830803033713</v>
       </c>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
     </row>
     <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57">
@@ -3045,9 +3070,12 @@
       <c r="C57">
         <v>28.132598451801307</v>
       </c>
-      <c r="D57" s="84">
+      <c r="D57" s="71">
         <v>35.042296598850157</v>
       </c>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
     </row>
     <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58">
@@ -3059,9 +3087,12 @@
       <c r="C58">
         <v>29.252699938151203</v>
       </c>
-      <c r="D58" s="84">
+      <c r="D58" s="71">
         <v>37.664670733960989</v>
       </c>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
     </row>
     <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59">
@@ -3073,9 +3104,12 @@
       <c r="C59">
         <v>38.233815949870618</v>
       </c>
-      <c r="D59" s="84">
+      <c r="D59" s="71">
         <v>50.73423033275192</v>
       </c>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
     </row>
     <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60">
@@ -3087,9 +3121,12 @@
       <c r="C60">
         <v>41.913057767373743</v>
       </c>
-      <c r="D60" s="84">
+      <c r="D60" s="71">
         <v>57.224897163583051</v>
       </c>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
     </row>
     <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61">
@@ -3101,9 +3138,12 @@
       <c r="C61">
         <v>46.140623298934813</v>
       </c>
-      <c r="D61" s="84">
+      <c r="D61" s="71">
         <v>61.893808574842218</v>
       </c>
+      <c r="E61" s="14"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="14"/>
     </row>
     <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62">
@@ -3118,6 +3158,24 @@
       <c r="D62" s="14">
         <v>62.95</v>
       </c>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="14"/>
+    </row>
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="14"/>
+    </row>
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F65" s="4"/>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F66" s="4"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -3209,7 +3267,7 @@
         <v>57</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -3233,7 +3291,7 @@
         <v>2007</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -3254,10 +3312,10 @@
     </row>
     <row r="4" spans="1:38" s="14" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
@@ -3285,7 +3343,7 @@
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
@@ -3329,13 +3387,13 @@
     </row>
     <row r="8" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="43">
         <v>0.2</v>
       </c>
-      <c r="C8" s="71" t="s">
-        <v>83</v>
+      <c r="C8" s="70" t="s">
+        <v>82</v>
       </c>
       <c r="D8" s="19">
         <v>0.151</v>
@@ -4296,10 +4354,10 @@
     </row>
     <row r="42" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="20"/>
-      <c r="B42" s="77"/>
-      <c r="C42" s="77"/>
-      <c r="D42" s="77"/>
-      <c r="E42" s="77"/>
+      <c r="B42" s="78"/>
+      <c r="C42" s="78"/>
+      <c r="D42" s="78"/>
+      <c r="E42" s="78"/>
       <c r="F42" s="19"/>
       <c r="J42" s="18"/>
       <c r="K42" s="18"/>
@@ -4313,22 +4371,22 @@
     <row r="43" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="26"/>
       <c r="B43" s="53"/>
-      <c r="C43" s="76" t="s">
+      <c r="C43" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="D43" s="74"/>
-      <c r="E43" s="74"/>
-      <c r="F43" s="75"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="75"/>
+      <c r="F43" s="76"/>
       <c r="G43" s="50"/>
       <c r="H43" s="26"/>
       <c r="I43" s="56"/>
-      <c r="J43" s="74" t="s">
+      <c r="J43" s="75" t="s">
         <v>61</v>
       </c>
-      <c r="K43" s="74"/>
-      <c r="L43" s="74"/>
-      <c r="M43" s="74"/>
-      <c r="N43" s="75"/>
+      <c r="K43" s="75"/>
+      <c r="L43" s="75"/>
+      <c r="M43" s="75"/>
+      <c r="N43" s="76"/>
       <c r="O43" s="26"/>
     </row>
     <row r="44" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
@@ -4378,7 +4436,7 @@
       <c r="AX44" s="16"/>
     </row>
     <row r="45" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="79" t="s">
+      <c r="A45" s="80" t="s">
         <v>0</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -4401,7 +4459,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G45" s="20"/>
-      <c r="H45" s="80" t="s">
+      <c r="H45" s="81" t="s">
         <v>0</v>
       </c>
       <c r="I45" s="2" t="s">
@@ -4429,7 +4487,7 @@
       <c r="AX45" s="15"/>
     </row>
     <row r="46" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="79"/>
+      <c r="A46" s="80"/>
       <c r="B46" s="2" t="s">
         <v>3</v>
       </c>
@@ -4450,7 +4508,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G46" s="20"/>
-      <c r="H46" s="81"/>
+      <c r="H46" s="82"/>
       <c r="I46" s="2" t="s">
         <v>3</v>
       </c>
@@ -4476,7 +4534,7 @@
       <c r="AX46" s="9"/>
     </row>
     <row r="47" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="79"/>
+      <c r="A47" s="80"/>
       <c r="B47" s="2" t="s">
         <v>4</v>
       </c>
@@ -4497,7 +4555,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G47" s="20"/>
-      <c r="H47" s="81"/>
+      <c r="H47" s="82"/>
       <c r="I47" s="2" t="s">
         <v>4</v>
       </c>
@@ -4523,7 +4581,7 @@
       <c r="AX47" s="9"/>
     </row>
     <row r="48" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="79"/>
+      <c r="A48" s="80"/>
       <c r="B48" s="2" t="s">
         <v>5</v>
       </c>
@@ -4544,7 +4602,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G48" s="20"/>
-      <c r="H48" s="81"/>
+      <c r="H48" s="82"/>
       <c r="I48" s="2" t="s">
         <v>5</v>
       </c>
@@ -4570,7 +4628,7 @@
       <c r="AX48" s="9"/>
     </row>
     <row r="49" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="79"/>
+      <c r="A49" s="80"/>
       <c r="B49" s="2" t="s">
         <v>6</v>
       </c>
@@ -4591,7 +4649,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G49" s="20"/>
-      <c r="H49" s="81"/>
+      <c r="H49" s="82"/>
       <c r="I49" s="2" t="s">
         <v>6</v>
       </c>
@@ -4616,7 +4674,7 @@
       </c>
     </row>
     <row r="50" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="79"/>
+      <c r="A50" s="80"/>
       <c r="B50" s="2" t="s">
         <v>7</v>
       </c>
@@ -4637,7 +4695,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G50" s="20"/>
-      <c r="H50" s="81"/>
+      <c r="H50" s="82"/>
       <c r="I50" s="2" t="s">
         <v>7</v>
       </c>
@@ -4662,7 +4720,7 @@
       </c>
     </row>
     <row r="51" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="79"/>
+      <c r="A51" s="80"/>
       <c r="B51" s="2" t="s">
         <v>13</v>
       </c>
@@ -4683,7 +4741,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G51" s="20"/>
-      <c r="H51" s="81"/>
+      <c r="H51" s="82"/>
       <c r="I51" s="2" t="s">
         <v>13</v>
       </c>
@@ -4708,7 +4766,7 @@
       </c>
     </row>
     <row r="52" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="79"/>
+      <c r="A52" s="80"/>
       <c r="B52" s="2" t="s">
         <v>8</v>
       </c>
@@ -4729,7 +4787,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G52" s="20"/>
-      <c r="H52" s="81"/>
+      <c r="H52" s="82"/>
       <c r="I52" s="2" t="s">
         <v>8</v>
       </c>
@@ -4754,7 +4812,7 @@
       </c>
     </row>
     <row r="53" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="79"/>
+      <c r="A53" s="80"/>
       <c r="B53" s="2" t="s">
         <v>9</v>
       </c>
@@ -4775,7 +4833,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G53" s="20"/>
-      <c r="H53" s="81"/>
+      <c r="H53" s="82"/>
       <c r="I53" s="2" t="s">
         <v>9</v>
       </c>
@@ -4800,7 +4858,7 @@
       </c>
     </row>
     <row r="54" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="79"/>
+      <c r="A54" s="80"/>
       <c r="B54" s="2" t="s">
         <v>10</v>
       </c>
@@ -4821,7 +4879,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G54" s="20"/>
-      <c r="H54" s="81"/>
+      <c r="H54" s="82"/>
       <c r="I54" s="2" t="s">
         <v>10</v>
       </c>
@@ -4846,7 +4904,7 @@
       </c>
     </row>
     <row r="55" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="79"/>
+      <c r="A55" s="80"/>
       <c r="B55" s="2" t="s">
         <v>11</v>
       </c>
@@ -4867,7 +4925,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G55" s="20"/>
-      <c r="H55" s="81"/>
+      <c r="H55" s="82"/>
       <c r="I55" s="2" t="s">
         <v>11</v>
       </c>
@@ -4892,7 +4950,7 @@
       </c>
     </row>
     <row r="56" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="79"/>
+      <c r="A56" s="80"/>
       <c r="B56" s="2" t="s">
         <v>12</v>
       </c>
@@ -4913,7 +4971,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G56" s="20"/>
-      <c r="H56" s="81"/>
+      <c r="H56" s="82"/>
       <c r="I56" s="2" t="s">
         <v>12</v>
       </c>
@@ -4938,7 +4996,7 @@
       </c>
     </row>
     <row r="57" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="79"/>
+      <c r="A57" s="80"/>
       <c r="B57" s="36" t="s">
         <v>36</v>
       </c>
@@ -4959,7 +5017,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G57" s="20"/>
-      <c r="H57" s="81"/>
+      <c r="H57" s="82"/>
       <c r="I57" s="36" t="s">
         <v>36</v>
       </c>
@@ -4984,7 +5042,7 @@
       </c>
     </row>
     <row r="58" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="79"/>
+      <c r="A58" s="80"/>
       <c r="B58" s="36" t="s">
         <v>37</v>
       </c>
@@ -5005,7 +5063,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G58" s="20"/>
-      <c r="H58" s="81"/>
+      <c r="H58" s="82"/>
       <c r="I58" s="36" t="s">
         <v>37</v>
       </c>
@@ -5030,7 +5088,7 @@
       </c>
     </row>
     <row r="59" spans="1:15" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="79"/>
+      <c r="A59" s="80"/>
       <c r="B59" s="36" t="s">
         <v>38</v>
       </c>
@@ -5051,7 +5109,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G59" s="20"/>
-      <c r="H59" s="81"/>
+      <c r="H59" s="82"/>
       <c r="I59" s="36" t="s">
         <v>38</v>
       </c>
@@ -5076,7 +5134,7 @@
       </c>
     </row>
     <row r="60" spans="1:15" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="79"/>
+      <c r="A60" s="80"/>
       <c r="B60" s="36" t="s">
         <v>39</v>
       </c>
@@ -5097,7 +5155,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G60" s="20"/>
-      <c r="H60" s="82"/>
+      <c r="H60" s="83"/>
       <c r="I60" s="36" t="s">
         <v>39</v>
       </c>
@@ -5139,7 +5197,7 @@
       <c r="O61" s="19"/>
     </row>
     <row r="62" spans="1:15" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="80" t="s">
+      <c r="A62" s="81" t="s">
         <v>1</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -5162,7 +5220,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G62" s="20"/>
-      <c r="H62" s="80" t="s">
+      <c r="H62" s="81" t="s">
         <v>1</v>
       </c>
       <c r="I62" s="2" t="s">
@@ -5189,7 +5247,7 @@
       </c>
     </row>
     <row r="63" spans="1:15" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="81"/>
+      <c r="A63" s="82"/>
       <c r="B63" s="2" t="s">
         <v>3</v>
       </c>
@@ -5210,7 +5268,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G63" s="20"/>
-      <c r="H63" s="81"/>
+      <c r="H63" s="82"/>
       <c r="I63" s="2" t="s">
         <v>3</v>
       </c>
@@ -5235,7 +5293,7 @@
       </c>
     </row>
     <row r="64" spans="1:15" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="81"/>
+      <c r="A64" s="82"/>
       <c r="B64" s="2" t="s">
         <v>4</v>
       </c>
@@ -5256,7 +5314,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G64" s="20"/>
-      <c r="H64" s="81"/>
+      <c r="H64" s="82"/>
       <c r="I64" s="2" t="s">
         <v>4</v>
       </c>
@@ -5281,7 +5339,7 @@
       </c>
     </row>
     <row r="65" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="81"/>
+      <c r="A65" s="82"/>
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
@@ -5302,7 +5360,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G65" s="20"/>
-      <c r="H65" s="81"/>
+      <c r="H65" s="82"/>
       <c r="I65" s="2" t="s">
         <v>5</v>
       </c>
@@ -5327,7 +5385,7 @@
       </c>
     </row>
     <row r="66" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="81"/>
+      <c r="A66" s="82"/>
       <c r="B66" s="2" t="s">
         <v>6</v>
       </c>
@@ -5348,7 +5406,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G66" s="20"/>
-      <c r="H66" s="81"/>
+      <c r="H66" s="82"/>
       <c r="I66" s="2" t="s">
         <v>6</v>
       </c>
@@ -5373,7 +5431,7 @@
       </c>
     </row>
     <row r="67" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="81"/>
+      <c r="A67" s="82"/>
       <c r="B67" s="2" t="s">
         <v>7</v>
       </c>
@@ -5394,7 +5452,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G67" s="20"/>
-      <c r="H67" s="81"/>
+      <c r="H67" s="82"/>
       <c r="I67" s="2" t="s">
         <v>7</v>
       </c>
@@ -5419,7 +5477,7 @@
       </c>
     </row>
     <row r="68" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="81"/>
+      <c r="A68" s="82"/>
       <c r="B68" s="2" t="s">
         <v>13</v>
       </c>
@@ -5440,7 +5498,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G68" s="20"/>
-      <c r="H68" s="81"/>
+      <c r="H68" s="82"/>
       <c r="I68" s="2" t="s">
         <v>13</v>
       </c>
@@ -5465,7 +5523,7 @@
       </c>
     </row>
     <row r="69" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="81"/>
+      <c r="A69" s="82"/>
       <c r="B69" s="2" t="s">
         <v>8</v>
       </c>
@@ -5486,7 +5544,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G69" s="20"/>
-      <c r="H69" s="81"/>
+      <c r="H69" s="82"/>
       <c r="I69" s="2" t="s">
         <v>8</v>
       </c>
@@ -5511,7 +5569,7 @@
       </c>
     </row>
     <row r="70" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="81"/>
+      <c r="A70" s="82"/>
       <c r="B70" s="2" t="s">
         <v>9</v>
       </c>
@@ -5532,7 +5590,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G70" s="20"/>
-      <c r="H70" s="81"/>
+      <c r="H70" s="82"/>
       <c r="I70" s="2" t="s">
         <v>9</v>
       </c>
@@ -5557,7 +5615,7 @@
       </c>
     </row>
     <row r="71" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="81"/>
+      <c r="A71" s="82"/>
       <c r="B71" s="2" t="s">
         <v>10</v>
       </c>
@@ -5578,7 +5636,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G71" s="20"/>
-      <c r="H71" s="81"/>
+      <c r="H71" s="82"/>
       <c r="I71" s="2" t="s">
         <v>10</v>
       </c>
@@ -5603,7 +5661,7 @@
       </c>
     </row>
     <row r="72" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="81"/>
+      <c r="A72" s="82"/>
       <c r="B72" s="2" t="s">
         <v>11</v>
       </c>
@@ -5624,7 +5682,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G72" s="20"/>
-      <c r="H72" s="81"/>
+      <c r="H72" s="82"/>
       <c r="I72" s="2" t="s">
         <v>11</v>
       </c>
@@ -5649,7 +5707,7 @@
       </c>
     </row>
     <row r="73" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="81"/>
+      <c r="A73" s="82"/>
       <c r="B73" s="2" t="s">
         <v>12</v>
       </c>
@@ -5670,7 +5728,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G73" s="20"/>
-      <c r="H73" s="81"/>
+      <c r="H73" s="82"/>
       <c r="I73" s="2" t="s">
         <v>12</v>
       </c>
@@ -5695,7 +5753,7 @@
       </c>
     </row>
     <row r="74" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="81"/>
+      <c r="A74" s="82"/>
       <c r="B74" s="36" t="s">
         <v>36</v>
       </c>
@@ -5716,7 +5774,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G74" s="20"/>
-      <c r="H74" s="81"/>
+      <c r="H74" s="82"/>
       <c r="I74" s="36" t="s">
         <v>36</v>
       </c>
@@ -5741,7 +5799,7 @@
       </c>
     </row>
     <row r="75" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="81"/>
+      <c r="A75" s="82"/>
       <c r="B75" s="36" t="s">
         <v>37</v>
       </c>
@@ -5762,7 +5820,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G75" s="20"/>
-      <c r="H75" s="81"/>
+      <c r="H75" s="82"/>
       <c r="I75" s="36" t="s">
         <v>37</v>
       </c>
@@ -5787,7 +5845,7 @@
       </c>
     </row>
     <row r="76" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="81"/>
+      <c r="A76" s="82"/>
       <c r="B76" s="36" t="s">
         <v>38</v>
       </c>
@@ -5808,7 +5866,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G76" s="20"/>
-      <c r="H76" s="81"/>
+      <c r="H76" s="82"/>
       <c r="I76" s="36" t="s">
         <v>38</v>
       </c>
@@ -5833,7 +5891,7 @@
       </c>
     </row>
     <row r="77" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="82"/>
+      <c r="A77" s="83"/>
       <c r="B77" s="36" t="s">
         <v>39</v>
       </c>
@@ -5854,7 +5912,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G77" s="20"/>
-      <c r="H77" s="82"/>
+      <c r="H77" s="83"/>
       <c r="I77" s="36" t="s">
         <v>39</v>
       </c>
@@ -5941,10 +5999,10 @@
     </row>
     <row r="81" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="19"/>
-      <c r="B81" s="77"/>
-      <c r="C81" s="77"/>
-      <c r="D81" s="77"/>
-      <c r="E81" s="77"/>
+      <c r="B81" s="78"/>
+      <c r="C81" s="78"/>
+      <c r="D81" s="78"/>
+      <c r="E81" s="78"/>
       <c r="F81" s="19"/>
       <c r="G81" s="48"/>
       <c r="H81" s="48"/>
@@ -5962,22 +6020,22 @@
     <row r="82" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="37"/>
       <c r="B82" s="37"/>
-      <c r="C82" s="83" t="s">
+      <c r="C82" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="D82" s="83"/>
-      <c r="E82" s="83"/>
-      <c r="F82" s="83"/>
+      <c r="D82" s="84"/>
+      <c r="E82" s="84"/>
+      <c r="F82" s="84"/>
       <c r="G82" s="20"/>
       <c r="H82" s="26"/>
       <c r="I82" s="56"/>
-      <c r="J82" s="74" t="s">
+      <c r="J82" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="K82" s="74"/>
-      <c r="L82" s="74"/>
-      <c r="M82" s="74"/>
-      <c r="N82" s="75"/>
+      <c r="K82" s="75"/>
+      <c r="L82" s="75"/>
+      <c r="M82" s="75"/>
+      <c r="N82" s="76"/>
       <c r="O82" s="26"/>
       <c r="P82" s="19"/>
       <c r="Q82" s="19"/>
@@ -6032,7 +6090,7 @@
       <c r="AB83" s="14"/>
     </row>
     <row r="84" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="79" t="s">
+      <c r="A84" s="80" t="s">
         <v>0</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -6055,7 +6113,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G84" s="48"/>
-      <c r="H84" s="80" t="s">
+      <c r="H84" s="81" t="s">
         <v>0</v>
       </c>
       <c r="I84" s="2" t="s">
@@ -6084,7 +6142,7 @@
       <c r="AB84" s="14"/>
     </row>
     <row r="85" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="79"/>
+      <c r="A85" s="80"/>
       <c r="B85" s="2" t="s">
         <v>3</v>
       </c>
@@ -6105,7 +6163,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G85" s="48"/>
-      <c r="H85" s="81"/>
+      <c r="H85" s="82"/>
       <c r="I85" s="2" t="s">
         <v>3</v>
       </c>
@@ -6132,7 +6190,7 @@
       <c r="AB85" s="14"/>
     </row>
     <row r="86" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="79"/>
+      <c r="A86" s="80"/>
       <c r="B86" s="2" t="s">
         <v>4</v>
       </c>
@@ -6153,7 +6211,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G86" s="48"/>
-      <c r="H86" s="81"/>
+      <c r="H86" s="82"/>
       <c r="I86" s="2" t="s">
         <v>4</v>
       </c>
@@ -6180,7 +6238,7 @@
       <c r="AB86" s="14"/>
     </row>
     <row r="87" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="79"/>
+      <c r="A87" s="80"/>
       <c r="B87" s="2" t="s">
         <v>5</v>
       </c>
@@ -6201,7 +6259,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G87" s="20"/>
-      <c r="H87" s="81"/>
+      <c r="H87" s="82"/>
       <c r="I87" s="2" t="s">
         <v>5</v>
       </c>
@@ -6228,7 +6286,7 @@
       <c r="AB87" s="14"/>
     </row>
     <row r="88" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="79"/>
+      <c r="A88" s="80"/>
       <c r="B88" s="2" t="s">
         <v>6</v>
       </c>
@@ -6249,7 +6307,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G88" s="48"/>
-      <c r="H88" s="81"/>
+      <c r="H88" s="82"/>
       <c r="I88" s="2" t="s">
         <v>6</v>
       </c>
@@ -6276,7 +6334,7 @@
       <c r="AB88" s="14"/>
     </row>
     <row r="89" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="79"/>
+      <c r="A89" s="80"/>
       <c r="B89" s="2" t="s">
         <v>7</v>
       </c>
@@ -6297,7 +6355,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G89" s="20"/>
-      <c r="H89" s="81"/>
+      <c r="H89" s="82"/>
       <c r="I89" s="2" t="s">
         <v>7</v>
       </c>
@@ -6325,7 +6383,7 @@
       <c r="AB89" s="14"/>
     </row>
     <row r="90" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="79"/>
+      <c r="A90" s="80"/>
       <c r="B90" s="2" t="s">
         <v>13</v>
       </c>
@@ -6346,7 +6404,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G90" s="48"/>
-      <c r="H90" s="81"/>
+      <c r="H90" s="82"/>
       <c r="I90" s="2" t="s">
         <v>13</v>
       </c>
@@ -6372,7 +6430,7 @@
       <c r="AB90" s="14"/>
     </row>
     <row r="91" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="79"/>
+      <c r="A91" s="80"/>
       <c r="B91" s="2" t="s">
         <v>8</v>
       </c>
@@ -6393,7 +6451,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G91" s="48"/>
-      <c r="H91" s="81"/>
+      <c r="H91" s="82"/>
       <c r="I91" s="2" t="s">
         <v>8</v>
       </c>
@@ -6419,7 +6477,7 @@
       <c r="AB91" s="14"/>
     </row>
     <row r="92" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" s="79"/>
+      <c r="A92" s="80"/>
       <c r="B92" s="2" t="s">
         <v>9</v>
       </c>
@@ -6440,7 +6498,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G92" s="48"/>
-      <c r="H92" s="81"/>
+      <c r="H92" s="82"/>
       <c r="I92" s="2" t="s">
         <v>9</v>
       </c>
@@ -6466,7 +6524,7 @@
       <c r="AB92" s="14"/>
     </row>
     <row r="93" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="79"/>
+      <c r="A93" s="80"/>
       <c r="B93" s="2" t="s">
         <v>10</v>
       </c>
@@ -6487,7 +6545,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G93" s="48"/>
-      <c r="H93" s="81"/>
+      <c r="H93" s="82"/>
       <c r="I93" s="2" t="s">
         <v>10</v>
       </c>
@@ -6513,7 +6571,7 @@
       <c r="AB93" s="14"/>
     </row>
     <row r="94" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="79"/>
+      <c r="A94" s="80"/>
       <c r="B94" s="2" t="s">
         <v>11</v>
       </c>
@@ -6534,7 +6592,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G94" s="20"/>
-      <c r="H94" s="81"/>
+      <c r="H94" s="82"/>
       <c r="I94" s="2" t="s">
         <v>11</v>
       </c>
@@ -6560,7 +6618,7 @@
       <c r="AB94" s="14"/>
     </row>
     <row r="95" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="79"/>
+      <c r="A95" s="80"/>
       <c r="B95" s="2" t="s">
         <v>12</v>
       </c>
@@ -6581,7 +6639,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G95" s="20"/>
-      <c r="H95" s="81"/>
+      <c r="H95" s="82"/>
       <c r="I95" s="2" t="s">
         <v>12</v>
       </c>
@@ -6609,7 +6667,7 @@
       <c r="AB95" s="14"/>
     </row>
     <row r="96" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="79"/>
+      <c r="A96" s="80"/>
       <c r="B96" s="36" t="s">
         <v>36</v>
       </c>
@@ -6630,7 +6688,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G96" s="20"/>
-      <c r="H96" s="81"/>
+      <c r="H96" s="82"/>
       <c r="I96" s="36" t="s">
         <v>36</v>
       </c>
@@ -6658,7 +6716,7 @@
       <c r="AB96" s="14"/>
     </row>
     <row r="97" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="79"/>
+      <c r="A97" s="80"/>
       <c r="B97" s="36" t="s">
         <v>37</v>
       </c>
@@ -6679,7 +6737,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G97" s="19"/>
-      <c r="H97" s="81"/>
+      <c r="H97" s="82"/>
       <c r="I97" s="36" t="s">
         <v>37</v>
       </c>
@@ -6707,7 +6765,7 @@
       <c r="AB97" s="14"/>
     </row>
     <row r="98" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="79"/>
+      <c r="A98" s="80"/>
       <c r="B98" s="36" t="s">
         <v>38</v>
       </c>
@@ -6728,7 +6786,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G98" s="19"/>
-      <c r="H98" s="81"/>
+      <c r="H98" s="82"/>
       <c r="I98" s="36" t="s">
         <v>38</v>
       </c>
@@ -6755,7 +6813,7 @@
       <c r="Q98" s="19"/>
     </row>
     <row r="99" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="79"/>
+      <c r="A99" s="80"/>
       <c r="B99" s="36" t="s">
         <v>39</v>
       </c>
@@ -6776,7 +6834,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G99" s="19"/>
-      <c r="H99" s="82"/>
+      <c r="H99" s="83"/>
       <c r="I99" s="36" t="s">
         <v>39</v>
       </c>
@@ -6822,7 +6880,7 @@
       <c r="Q100" s="19"/>
     </row>
     <row r="101" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="80" t="s">
+      <c r="A101" s="81" t="s">
         <v>1</v>
       </c>
       <c r="B101" s="2" t="s">
@@ -6845,7 +6903,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G101" s="19"/>
-      <c r="H101" s="80" t="s">
+      <c r="H101" s="81" t="s">
         <v>1</v>
       </c>
       <c r="I101" s="2" t="s">
@@ -6874,7 +6932,7 @@
       <c r="Q101" s="19"/>
     </row>
     <row r="102" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A102" s="81"/>
+      <c r="A102" s="82"/>
       <c r="B102" s="2" t="s">
         <v>3</v>
       </c>
@@ -6895,7 +6953,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G102" s="19"/>
-      <c r="H102" s="81"/>
+      <c r="H102" s="82"/>
       <c r="I102" s="2" t="s">
         <v>3</v>
       </c>
@@ -6922,7 +6980,7 @@
       <c r="Q102" s="19"/>
     </row>
     <row r="103" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="81"/>
+      <c r="A103" s="82"/>
       <c r="B103" s="2" t="s">
         <v>4</v>
       </c>
@@ -6943,7 +7001,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G103" s="19"/>
-      <c r="H103" s="81"/>
+      <c r="H103" s="82"/>
       <c r="I103" s="2" t="s">
         <v>4</v>
       </c>
@@ -6970,7 +7028,7 @@
       <c r="Q103" s="19"/>
     </row>
     <row r="104" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="81"/>
+      <c r="A104" s="82"/>
       <c r="B104" s="2" t="s">
         <v>5</v>
       </c>
@@ -6991,7 +7049,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G104" s="19"/>
-      <c r="H104" s="81"/>
+      <c r="H104" s="82"/>
       <c r="I104" s="2" t="s">
         <v>5</v>
       </c>
@@ -7018,7 +7076,7 @@
       <c r="Q104" s="19"/>
     </row>
     <row r="105" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="81"/>
+      <c r="A105" s="82"/>
       <c r="B105" s="2" t="s">
         <v>6</v>
       </c>
@@ -7039,7 +7097,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G105" s="19"/>
-      <c r="H105" s="81"/>
+      <c r="H105" s="82"/>
       <c r="I105" s="2" t="s">
         <v>6</v>
       </c>
@@ -7066,7 +7124,7 @@
       <c r="Q105" s="19"/>
     </row>
     <row r="106" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="81"/>
+      <c r="A106" s="82"/>
       <c r="B106" s="2" t="s">
         <v>7</v>
       </c>
@@ -7087,7 +7145,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G106" s="19"/>
-      <c r="H106" s="81"/>
+      <c r="H106" s="82"/>
       <c r="I106" s="2" t="s">
         <v>7</v>
       </c>
@@ -7114,7 +7172,7 @@
       <c r="Q106" s="19"/>
     </row>
     <row r="107" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="81"/>
+      <c r="A107" s="82"/>
       <c r="B107" s="2" t="s">
         <v>13</v>
       </c>
@@ -7135,7 +7193,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G107" s="19"/>
-      <c r="H107" s="81"/>
+      <c r="H107" s="82"/>
       <c r="I107" s="2" t="s">
         <v>13</v>
       </c>
@@ -7162,7 +7220,7 @@
       <c r="Q107" s="19"/>
     </row>
     <row r="108" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A108" s="81"/>
+      <c r="A108" s="82"/>
       <c r="B108" s="2" t="s">
         <v>8</v>
       </c>
@@ -7183,7 +7241,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G108" s="19"/>
-      <c r="H108" s="81"/>
+      <c r="H108" s="82"/>
       <c r="I108" s="2" t="s">
         <v>8</v>
       </c>
@@ -7210,7 +7268,7 @@
       <c r="Q108" s="19"/>
     </row>
     <row r="109" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A109" s="81"/>
+      <c r="A109" s="82"/>
       <c r="B109" s="2" t="s">
         <v>9</v>
       </c>
@@ -7231,7 +7289,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G109" s="19"/>
-      <c r="H109" s="81"/>
+      <c r="H109" s="82"/>
       <c r="I109" s="2" t="s">
         <v>9</v>
       </c>
@@ -7258,7 +7316,7 @@
       <c r="Q109" s="19"/>
     </row>
     <row r="110" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A110" s="81"/>
+      <c r="A110" s="82"/>
       <c r="B110" s="2" t="s">
         <v>10</v>
       </c>
@@ -7279,7 +7337,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G110" s="19"/>
-      <c r="H110" s="81"/>
+      <c r="H110" s="82"/>
       <c r="I110" s="2" t="s">
         <v>10</v>
       </c>
@@ -7306,7 +7364,7 @@
       <c r="Q110" s="19"/>
     </row>
     <row r="111" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="81"/>
+      <c r="A111" s="82"/>
       <c r="B111" s="2" t="s">
         <v>11</v>
       </c>
@@ -7327,7 +7385,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G111" s="19"/>
-      <c r="H111" s="81"/>
+      <c r="H111" s="82"/>
       <c r="I111" s="2" t="s">
         <v>11</v>
       </c>
@@ -7354,7 +7412,7 @@
       <c r="Q111" s="19"/>
     </row>
     <row r="112" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A112" s="81"/>
+      <c r="A112" s="82"/>
       <c r="B112" s="2" t="s">
         <v>12</v>
       </c>
@@ -7375,7 +7433,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G112" s="19"/>
-      <c r="H112" s="81"/>
+      <c r="H112" s="82"/>
       <c r="I112" s="2" t="s">
         <v>12</v>
       </c>
@@ -7402,7 +7460,7 @@
       <c r="Q112" s="19"/>
     </row>
     <row r="113" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="81"/>
+      <c r="A113" s="82"/>
       <c r="B113" s="36" t="s">
         <v>36</v>
       </c>
@@ -7423,7 +7481,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G113" s="19"/>
-      <c r="H113" s="81"/>
+      <c r="H113" s="82"/>
       <c r="I113" s="36" t="s">
         <v>36</v>
       </c>
@@ -7450,7 +7508,7 @@
       <c r="Q113" s="19"/>
     </row>
     <row r="114" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A114" s="81"/>
+      <c r="A114" s="82"/>
       <c r="B114" s="36" t="s">
         <v>37</v>
       </c>
@@ -7471,7 +7529,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G114" s="19"/>
-      <c r="H114" s="81"/>
+      <c r="H114" s="82"/>
       <c r="I114" s="36" t="s">
         <v>37</v>
       </c>
@@ -7498,7 +7556,7 @@
       <c r="Q114" s="19"/>
     </row>
     <row r="115" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A115" s="81"/>
+      <c r="A115" s="82"/>
       <c r="B115" s="36" t="s">
         <v>38</v>
       </c>
@@ -7519,7 +7577,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G115" s="19"/>
-      <c r="H115" s="81"/>
+      <c r="H115" s="82"/>
       <c r="I115" s="36" t="s">
         <v>38</v>
       </c>
@@ -7546,7 +7604,7 @@
       <c r="Q115" s="19"/>
     </row>
     <row r="116" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A116" s="82"/>
+      <c r="A116" s="83"/>
       <c r="B116" s="36" t="s">
         <v>39</v>
       </c>
@@ -7567,7 +7625,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G116" s="14"/>
-      <c r="H116" s="82"/>
+      <c r="H116" s="83"/>
       <c r="I116" s="36" t="s">
         <v>39</v>
       </c>
@@ -8306,8 +8364,8 @@
       <c r="W145" s="9"/>
     </row>
     <row r="146" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A146" s="78"/>
-      <c r="B146" s="78"/>
+      <c r="A146" s="79"/>
+      <c r="B146" s="79"/>
       <c r="C146" s="27"/>
       <c r="D146" s="27"/>
       <c r="E146" s="27"/>
@@ -8431,8 +8489,8 @@
       <c r="W150" s="9"/>
     </row>
     <row r="151" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A151" s="78"/>
-      <c r="B151" s="78"/>
+      <c r="A151" s="79"/>
+      <c r="B151" s="79"/>
       <c r="C151" s="27"/>
       <c r="D151" s="27"/>
       <c r="E151" s="27"/>

</xml_diff>

<commit_message>
update epsA and epsR
</commit_message>
<xml_diff>
--- a/Config/HIV_parameters_Kenya.xlsx
+++ b/Config/HIV_parameters_Kenya.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20364"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20366"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Kenya_model_HPV-HIVacq\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968F9791-A00C-4538-A7E9-605E66BE1F17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8992FDD6-287D-485D-A615-9A83A4E11A71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="5955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Protection" sheetId="5" r:id="rId1"/>
@@ -775,6 +775,72 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>42333</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1112307</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB9BAA39-1B4E-48C5-8B76-62995FB241F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8731249" y="9091083"/>
+          <a:ext cx="5737225" cy="4754034"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1041,8 +1107,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AI66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2121,7 +2187,7 @@
         <v>2.9059037050679932</v>
       </c>
       <c r="C34" s="64">
-        <f t="shared" ref="C34:C42" si="0">0.74*B34</f>
+        <f t="shared" ref="C34:C38" si="0">0.74*B34</f>
         <v>2.1503687417503148</v>
       </c>
       <c r="D34" s="14" t="s">
@@ -2329,8 +2395,8 @@
         <v>23.03933533384064</v>
       </c>
       <c r="C38" s="64">
-        <f t="shared" si="0"/>
-        <v>17.049108147042073</v>
+        <f>0.85*B38</f>
+        <v>19.583435033764545</v>
       </c>
       <c r="D38" t="s">
         <v>74</v>
@@ -2381,8 +2447,8 @@
         <v>31.39083758325436</v>
       </c>
       <c r="C39" s="64">
-        <f t="shared" si="0"/>
-        <v>23.229219811608225</v>
+        <f t="shared" ref="C39:C46" si="1">0.85*B39</f>
+        <v>26.682211945766205</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>74</v>
@@ -2432,8 +2498,8 @@
         <v>35.323435905602842</v>
       </c>
       <c r="C40" s="64">
-        <f t="shared" si="0"/>
-        <v>26.139342570146102</v>
+        <f t="shared" si="1"/>
+        <v>30.024920519762414</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>74</v>
@@ -2483,8 +2549,8 @@
         <v>38.706882519484815</v>
       </c>
       <c r="C41" s="64">
-        <f t="shared" si="0"/>
-        <v>28.643093064418764</v>
+        <f t="shared" si="1"/>
+        <v>32.900850141562088</v>
       </c>
       <c r="D41" t="s">
         <v>73</v>
@@ -2538,8 +2604,8 @@
         <v>44.4</v>
       </c>
       <c r="C42" s="64">
-        <f>I42</f>
-        <v>36.555703999999999</v>
+        <f t="shared" si="1"/>
+        <v>37.739999999999995</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>75</v>
@@ -2554,7 +2620,8 @@
         <v>49.4</v>
       </c>
       <c r="I42" s="14">
-        <v>36.555703999999999</v>
+        <f>0.75*H42</f>
+        <v>37.049999999999997</v>
       </c>
       <c r="J42" s="14"/>
       <c r="K42" s="14"/>
@@ -2592,11 +2659,12 @@
         <v>2015</v>
       </c>
       <c r="B43" s="68">
-        <f t="shared" ref="B43:B46" si="1">H43-5</f>
+        <f t="shared" ref="B43:B46" si="2">H43-5</f>
         <v>44.764000000000003</v>
       </c>
       <c r="C43" s="64">
-        <v>38.454000000000001</v>
+        <f t="shared" si="1"/>
+        <v>38.049399999999999</v>
       </c>
       <c r="D43" t="s">
         <v>77</v>
@@ -2649,11 +2717,12 @@
         <v>2016</v>
       </c>
       <c r="B44" s="68">
+        <f t="shared" si="2"/>
+        <v>54.2</v>
+      </c>
+      <c r="C44" s="64">
         <f t="shared" si="1"/>
-        <v>54.2</v>
-      </c>
-      <c r="C44" s="64">
-        <v>44.800000000000004</v>
+        <v>46.07</v>
       </c>
       <c r="D44" t="s">
         <v>78</v>
@@ -2706,11 +2775,12 @@
         <v>2017</v>
       </c>
       <c r="B45" s="68">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="C45" s="64">
         <f t="shared" si="1"/>
-        <v>63</v>
-      </c>
-      <c r="C45" s="64">
-        <v>51.85</v>
+        <v>53.55</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>78</v>
@@ -2763,11 +2833,12 @@
         <v>2018</v>
       </c>
       <c r="B46" s="68">
+        <f t="shared" si="2"/>
+        <v>62.95</v>
+      </c>
+      <c r="C46" s="64">
         <f t="shared" si="1"/>
-        <v>62.95</v>
-      </c>
-      <c r="C46" s="13">
-        <v>53.631</v>
+        <v>53.5075</v>
       </c>
       <c r="D46" t="s">
         <v>76</v>
@@ -2871,10 +2942,17 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <v>1.6980612730897779</v>
+        <v>0</v>
       </c>
       <c r="D49" s="71">
         <v>1.3083920290325319</v>
+      </c>
+      <c r="F49" s="14">
+        <v>1.1320408487265186</v>
+      </c>
+      <c r="H49">
+        <f>I42/H42</f>
+        <v>0.75</v>
       </c>
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
@@ -2904,13 +2982,19 @@
         <v>0.11943150603129105</v>
       </c>
       <c r="C50">
-        <v>3.7967333204294031</v>
+        <v>2.1503687417503148</v>
       </c>
       <c r="D50" s="71">
         <v>2.9059037050679932</v>
       </c>
       <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
+      <c r="F50" s="14">
+        <v>2.5311555469529354</v>
+      </c>
+      <c r="H50" s="14">
+        <f t="shared" ref="H50:H53" si="3">I43/H43</f>
+        <v>0.77272727272727271</v>
+      </c>
       <c r="T50" s="4"/>
       <c r="U50" s="4"/>
       <c r="V50" s="4"/>
@@ -2936,14 +3020,20 @@
         <v>1.0854341736694677</v>
       </c>
       <c r="C51">
-        <v>8.6200480817215688</v>
+        <v>4.8592105160631771</v>
       </c>
       <c r="D51" s="71">
         <v>6.5665006973826721</v>
       </c>
       <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
+      <c r="F51" s="14">
+        <v>5.7466987211477125</v>
+      </c>
       <c r="G51" s="14"/>
+      <c r="H51" s="14">
+        <f t="shared" si="3"/>
+        <v>0.75675675675675669</v>
+      </c>
       <c r="L51" s="14"/>
       <c r="M51" s="71"/>
       <c r="N51" s="71"/>
@@ -2975,14 +3065,20 @@
         <v>4.7345437830383821</v>
       </c>
       <c r="C52">
-        <v>12.094549993791215</v>
+        <v>6.8048232456990858</v>
       </c>
       <c r="D52" s="71">
         <v>9.1957070887825481</v>
       </c>
       <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
+      <c r="F52" s="14">
+        <v>8.063033329194143</v>
+      </c>
       <c r="G52" s="14"/>
+      <c r="H52" s="14">
+        <f t="shared" si="3"/>
+        <v>0.76250000000000007</v>
+      </c>
     </row>
     <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53">
@@ -2992,15 +3088,20 @@
         <v>8.0786986150802385</v>
       </c>
       <c r="C53">
-        <v>16.440054062132464</v>
+        <v>9.252632886367989</v>
       </c>
       <c r="D53" s="71">
         <v>12.503557954551336</v>
       </c>
       <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
+      <c r="F53" s="14">
+        <v>10.960036041421644</v>
+      </c>
       <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
+      <c r="H53" s="14">
+        <f t="shared" si="3"/>
+        <v>0.78927152317880789</v>
+      </c>
       <c r="I53" s="14"/>
     </row>
     <row r="54" spans="1:35" x14ac:dyDescent="0.25">
@@ -3011,13 +3112,16 @@
         <v>23.03933533384064</v>
       </c>
       <c r="C54">
-        <v>22.220695539853899</v>
+        <v>17.049108147042073</v>
       </c>
       <c r="D54" s="71">
-        <v>16.96536733473387</v>
+        <f>0.85*B54</f>
+        <v>19.583435033764545</v>
       </c>
       <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
+      <c r="F54" s="14">
+        <v>14.813797026569265</v>
+      </c>
       <c r="G54" s="14"/>
       <c r="H54" s="14"/>
       <c r="I54" s="14"/>
@@ -3030,13 +3134,16 @@
         <v>31.39083758325436</v>
       </c>
       <c r="C55">
-        <v>27.1560777865852</v>
+        <v>23.543128187440772</v>
       </c>
       <c r="D55" s="71">
-        <v>22.691288338593512</v>
+        <f t="shared" ref="D55:D62" si="4">0.85*B55</f>
+        <v>26.682211945766205</v>
       </c>
       <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
+      <c r="F55" s="14">
+        <v>21.724862229268158</v>
+      </c>
       <c r="G55" s="14"/>
       <c r="H55" s="14"/>
       <c r="I55" s="14"/>
@@ -3049,13 +3156,16 @@
         <v>35.323435905602842</v>
       </c>
       <c r="C56">
-        <v>25.676713341272123</v>
+        <v>26.49257692920213</v>
       </c>
       <c r="D56" s="71">
-        <v>32.132830803033713</v>
+        <f t="shared" si="4"/>
+        <v>30.024920519762414</v>
       </c>
       <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
+      <c r="F56" s="14">
+        <v>22.253151562435839</v>
+      </c>
       <c r="G56" s="14"/>
       <c r="H56" s="14"/>
       <c r="I56" s="14"/>
@@ -3068,13 +3178,16 @@
         <v>38.706882519484815</v>
       </c>
       <c r="C57">
+        <v>29.030161889613609</v>
+      </c>
+      <c r="D57" s="71">
+        <f t="shared" si="4"/>
+        <v>32.900850141562088</v>
+      </c>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14">
         <v>28.132598451801307</v>
       </c>
-      <c r="D57" s="71">
-        <v>35.042296598850157</v>
-      </c>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
       <c r="G57" s="14"/>
     </row>
     <row r="58" spans="1:35" x14ac:dyDescent="0.25">
@@ -3085,13 +3198,16 @@
         <v>44.4</v>
       </c>
       <c r="C58">
+        <v>37.049999999999997</v>
+      </c>
+      <c r="D58" s="71">
+        <f t="shared" si="4"/>
+        <v>37.739999999999995</v>
+      </c>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14">
         <v>29.252699938151203</v>
       </c>
-      <c r="D58" s="71">
-        <v>37.664670733960989</v>
-      </c>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
       <c r="G58" s="14"/>
     </row>
     <row r="59" spans="1:35" x14ac:dyDescent="0.25">
@@ -3102,13 +3218,16 @@
         <v>44.764000000000003</v>
       </c>
       <c r="C59">
-        <v>38.233815949870618</v>
+        <v>38.454000000000001</v>
       </c>
       <c r="D59" s="71">
-        <v>50.73423033275192</v>
+        <f t="shared" si="4"/>
+        <v>38.049399999999999</v>
       </c>
       <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
+      <c r="F59" s="4">
+        <v>32.00666180174666</v>
+      </c>
       <c r="G59" s="14"/>
     </row>
     <row r="60" spans="1:35" x14ac:dyDescent="0.25">
@@ -3119,13 +3238,16 @@
         <v>54.2</v>
       </c>
       <c r="C60">
-        <v>41.913057767373743</v>
+        <v>44.800000000000004</v>
       </c>
       <c r="D60" s="71">
-        <v>57.224897163583051</v>
+        <f t="shared" si="4"/>
+        <v>46.07</v>
       </c>
       <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
+      <c r="F60" s="4">
+        <v>38.233815949870618</v>
+      </c>
       <c r="G60" s="14"/>
     </row>
     <row r="61" spans="1:35" x14ac:dyDescent="0.25">
@@ -3136,13 +3258,16 @@
         <v>63</v>
       </c>
       <c r="C61">
-        <v>46.140623298934813</v>
+        <v>51.85</v>
       </c>
       <c r="D61" s="71">
-        <v>61.893808574842218</v>
+        <f t="shared" si="4"/>
+        <v>53.55</v>
       </c>
       <c r="E61" s="14"/>
-      <c r="F61" s="4"/>
+      <c r="F61" s="4">
+        <v>41.913057767373743</v>
+      </c>
       <c r="G61" s="14"/>
     </row>
     <row r="62" spans="1:35" x14ac:dyDescent="0.25">
@@ -3155,11 +3280,14 @@
       <c r="C62">
         <v>53.631</v>
       </c>
-      <c r="D62" s="14">
-        <v>62.95</v>
+      <c r="D62" s="71">
+        <f t="shared" si="4"/>
+        <v>53.5075</v>
       </c>
       <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
+      <c r="F62" s="4">
+        <v>46.140623298934813</v>
+      </c>
       <c r="G62" s="14"/>
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.25">
@@ -3185,6 +3313,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
test runs for stochastic mod
</commit_message>
<xml_diff>
--- a/Config/HIV_parameters_Kenya.xlsx
+++ b/Config/HIV_parameters_Kenya.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Kenya_model_HPV-HIVacq\HHCoM\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Kenya_model_HPV-HIVacq\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8992FDD6-287D-485D-A615-9A83A4E11A71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FABACB-B4CA-43E1-B85D-033F605247B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Protection" sheetId="5" r:id="rId1"/>
@@ -1107,8 +1107,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AI66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,7 +1710,7 @@
         <v>26</v>
       </c>
       <c r="B18" s="22">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C18" s="26"/>
       <c r="D18" s="26"/>
@@ -2187,7 +2187,7 @@
         <v>2.9059037050679932</v>
       </c>
       <c r="C34" s="64">
-        <f t="shared" ref="C34:C38" si="0">0.74*B34</f>
+        <f t="shared" ref="C34:C37" si="0">0.74*B34</f>
         <v>2.1503687417503148</v>
       </c>
       <c r="D34" s="14" t="s">

</xml_diff>